<commit_message>
print date in template, template css adaptations
</commit_message>
<xml_diff>
--- a/collected.xlsx
+++ b/collected.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>nombres</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>rick grimes</t>
+  </si>
+  <si>
+    <t>marca</t>
+  </si>
+  <si>
+    <t>maestro</t>
+  </si>
+  <si>
+    <t>sodimac</t>
   </si>
 </sst>
 </file>
@@ -421,15 +430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,28 +449,31 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -472,28 +484,31 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
       <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -504,28 +519,31 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
       </c>
       <c r="J3" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -536,24 +554,27 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
       <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
-        <v>7</v>
-      </c>
       <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>